<commit_message>
Need to write final conclusions
</commit_message>
<xml_diff>
--- a/Assignments/Project3/P3_Data.xlsx
+++ b/Assignments/Project3/P3_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97ECFD3-719A-4CDE-9BE4-8114D51F13D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477B5DF6-99D0-44FD-99B3-3CDF25F0DED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{09D6966A-56E8-4463-9806-8089B6ACFC20}"/>
   </bookViews>
@@ -207,9 +207,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="174" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -284,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,18 +329,24 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,62 +379,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Traffic Load - Network A</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -721,37 +673,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -2157,15 +2079,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>7328</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>7328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2535,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5472FA95-8779-4D51-BF62-F3B98DB8077F}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,15 +2474,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2790,6 +2712,14 @@
       <c r="F11">
         <v>10</v>
       </c>
+      <c r="H11">
+        <f>G3*1000</f>
+        <v>200</v>
+      </c>
+      <c r="K11">
+        <f>K3*1000</f>
+        <v>333.33333333333331</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -2798,6 +2728,14 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H16" si="1">G4*1000</f>
+        <v>400</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:K16" si="2">K4*1000</f>
+        <v>666.66666666666663</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -2813,6 +2751,14 @@
       <c r="F13" t="s">
         <v>49</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>666.66666666666663</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2826,8 +2772,16 @@
         <v>46</v>
       </c>
       <c r="F14">
-        <f>G3+0.5*(0.06+G4+0.5*(0.04+G6)+0.3*(0.03+G8))+0.5*(0.05+G5+0.3*(0.02+G8)+0.4*(0.01+G7))</f>
-        <v>0.79761688311688306</v>
+        <f>SUMPRODUCT(C13:C17,C21:C25)</f>
+        <v>0.79761688311688317</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>173.91304347826087</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2842,8 +2796,16 @@
         <v>48</v>
       </c>
       <c r="F15">
-        <f>K3+0.5*(0.06+K4+0.5*(0.04+K6)+0.3*(0.03+K8))+0.5*(0.05+K5+0.3*(0.02+G9)+0.4*(0.01+K7))</f>
-        <v>1.1788935360705546</v>
+        <f>SUMPRODUCT(D21:D25,C13:C17)</f>
+        <v>1.2095057809685137</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>151.51515151515153</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2854,6 +2816,14 @@
         <v>0.3</v>
       </c>
       <c r="D16" s="4"/>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>181.81818181818181</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>204.08163265306121</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -2865,11 +2835,11 @@
       <c r="D17" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
@@ -2886,11 +2856,11 @@
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="25">
         <f>G3+0.06+G4</f>
         <v>0.66</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="25">
         <f>K3+0.06+K4</f>
         <v>1.06</v>
       </c>
@@ -2899,11 +2869,11 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="25">
         <f>G3+0.05+G5</f>
         <v>0.65</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="25">
         <f>K3+0.05+K5</f>
         <v>1.0499999999999998</v>
       </c>
@@ -2912,7 +2882,7 @@
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="25">
         <f>G3+0.06+G4+0.04+G6</f>
         <v>0.8600000000000001</v>
       </c>
@@ -2958,10 +2928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC06F7B-4B30-41AA-A5D1-AEF115CE92AD}">
-  <dimension ref="B1:O17"/>
+  <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,7 +3253,7 @@
       <c r="L12">
         <v>0.66</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="28">
         <f>ABS((L12-K12)/L12)</f>
         <v>7.406400665190624E-5</v>
       </c>
@@ -3311,7 +3281,7 @@
       <c r="L13">
         <v>0.65</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="28">
         <f t="shared" ref="M13:M17" si="2">ABS((L13-K13)/L13)</f>
         <v>1.4389667262820333E-3</v>
       </c>
@@ -3339,7 +3309,7 @@
       <c r="L14">
         <v>0.8600000000000001</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="28">
         <f t="shared" si="2"/>
         <v>1.0489855924386753E-3</v>
       </c>
@@ -3367,7 +3337,7 @@
       <c r="L15">
         <v>0.86181818181818182</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="28">
         <f t="shared" si="2"/>
         <v>3.82567969387508E-3</v>
       </c>
@@ -3395,10 +3365,11 @@
       <c r="L16" s="12">
         <v>0.80285714285714294</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="29">
         <f t="shared" si="2"/>
         <v>4.0968483666518523E-3</v>
       </c>
+      <c r="N16" s="26"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
@@ -3424,9 +3395,15 @@
         <f>SUMPRODUCT(L12:L16,O3:O7)</f>
         <v>0.79761688311688317</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="30">
         <f t="shared" si="2"/>
         <v>2.5770954611263833E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="26">
+        <f>AVERAGE(M12:M16)</f>
+        <v>2.0969088771799092E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3437,10 +3414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752A21F7-07F8-4DA3-997C-BEFBEAB2554C}">
-  <dimension ref="B2:O18"/>
+  <dimension ref="B2:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:H18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3906,7 +3883,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="J18" s="6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="K18" s="19">
         <f>SUMPRODUCT(K13:K17,L4:L8)</f>
@@ -3919,6 +3896,12 @@
       <c r="M18" s="21">
         <f t="shared" si="3"/>
         <v>8.2212653635365326E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="27">
+        <f>AVERAGE(M13:M17)</f>
+        <v>8.9297445694615715E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished all but conclusion
</commit_message>
<xml_diff>
--- a/Assignments/Project3/P3_Data.xlsx
+++ b/Assignments/Project3/P3_Data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F7F81C-91BA-4ADF-B1FB-92A0D0E0A3D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF2A36C-A51A-4165-A297-76B4F85ED31E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{09D6966A-56E8-4463-9806-8089B6ACFC20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{09D6966A-56E8-4463-9806-8089B6ACFC20}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpectedDelay" sheetId="4" r:id="rId1"/>
-    <sheet name="NetA" sheetId="2" r:id="rId2"/>
-    <sheet name="NetB" sheetId="3" r:id="rId3"/>
+    <sheet name="NetA_lifetime_load" sheetId="2" r:id="rId2"/>
+    <sheet name="NetB_lifetime_load" sheetId="3" r:id="rId3"/>
+    <sheet name="NetA_queues" sheetId="5" r:id="rId4"/>
+    <sheet name="NetB_queues" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="60">
   <si>
     <t>B</t>
   </si>
@@ -198,16 +200,27 @@
   </si>
   <si>
     <t>Expected time in system for Nodes A-F:</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Nodetime</t>
+  </si>
+  <si>
+    <t>Service Time:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -266,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -292,12 +305,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,12 +443,50 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +685,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>NetA!$N$3:$N$7</c:f>
+              <c:f>NetA_lifetime_load!$N$3:$N$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -580,7 +708,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>NetA!$L$3:$L$7</c:f>
+              <c:f>NetA_lifetime_load!$L$3:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -854,7 +982,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>NetB!$J$4:$J$8</c:f>
+              <c:f>NetB_lifetime_load!$J$4:$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -877,7 +1005,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>NetB!$L$4:$L$8</c:f>
+              <c:f>NetB_lifetime_load!$L$4:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2467,10 +2595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5472FA95-8779-4D51-BF62-F3B98DB8077F}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,15 +2614,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2790,7 +2918,7 @@
         <v>44</v>
       </c>
       <c r="F14">
-        <f>SUMPRODUCT(C13:C17,C21:C25)</f>
+        <f>SUMPRODUCT(C13:C17,C22:C26)</f>
         <v>0.79761688311688317</v>
       </c>
       <c r="H14">
@@ -2814,7 +2942,7 @@
         <v>46</v>
       </c>
       <c r="F15">
-        <f>SUMPRODUCT(D21:D25,C13:C17)</f>
+        <f>SUMPRODUCT(D22:D26,C13:C17)</f>
         <v>1.2095057809685137</v>
       </c>
       <c r="H15">
@@ -2853,11 +2981,11 @@
       <c r="D17" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
@@ -2872,65 +3000,78 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <f>G3</f>
+        <v>0.2</v>
+      </c>
+      <c r="D21">
+        <f>K3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C22" s="23">
         <f>G3+0.06+G4</f>
         <v>0.66</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D22" s="23">
         <f>K3+0.06+K4</f>
         <v>1.06</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C23" s="23">
         <f>G3+0.05+G5</f>
         <v>0.65</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D23" s="23">
         <f>K3+0.05+K5</f>
         <v>1.0499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C24" s="23">
         <f>G3+0.06+G4+0.04+G6</f>
         <v>0.8600000000000001</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <f>K3+0.06+K4+0.04+K6</f>
         <v>1.2739130434782608</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>0.5*(G3+0.06+G4+0.03+G8)+0.5*(G3+0.05+G5+0.02+G8)</f>
         <v>0.86181818181818182</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f>0.5*(K3+0.06+K4+0.03+K8)+0.5*(K3+0.05+K5+0.02+K8)</f>
         <v>1.2840816326530611</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>G3+0.05+G5+0.01+G7</f>
         <v>0.80285714285714294</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f>K3+0.05+K5+0.01+K7</f>
         <v>1.2115151515151514</v>
       </c>
@@ -2949,7 +3090,7 @@
   <dimension ref="B1:O19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +3098,7 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
@@ -3293,14 +3435,14 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K16" si="1">AVERAGEIF(D4:D18, J13,F4:F18)</f>
+        <f>AVERAGEIF(D4:D18, J13,F4:F18)</f>
         <v>0.65093532837208334</v>
       </c>
       <c r="L13">
         <v>0.65</v>
       </c>
       <c r="M13" s="26">
-        <f t="shared" ref="M13:M17" si="2">ABS((L13-K13)/L13)</f>
+        <f t="shared" ref="M13:M17" si="1">ABS((L13-K13)/L13)</f>
         <v>1.4389667262820333E-3</v>
       </c>
     </row>
@@ -3321,14 +3463,14 @@
         <v>2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f>AVERAGEIF(D5:D18, J14,F5:F19)</f>
         <v>0.86090212760949736</v>
       </c>
       <c r="L14">
         <v>0.8600000000000001</v>
       </c>
       <c r="M14" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0489855924386753E-3</v>
       </c>
     </row>
@@ -3349,14 +3491,14 @@
         <v>3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f>AVERAGEIF(D6:D18, J15,F6:F20)</f>
         <v>0.86511522213617598</v>
       </c>
       <c r="L15">
         <v>0.86181818181818182</v>
       </c>
       <c r="M15" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.82567969387508E-3</v>
       </c>
     </row>
@@ -3377,14 +3519,14 @@
         <v>4</v>
       </c>
       <c r="K16" s="12">
-        <f t="shared" si="1"/>
+        <f>AVERAGEIF(D7:D18, J16,F7:F21)</f>
         <v>0.80614632683151199</v>
       </c>
       <c r="L16" s="12">
         <v>0.80285714285714294</v>
       </c>
       <c r="M16" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.0968483666518523E-3</v>
       </c>
       <c r="N16" s="24"/>
@@ -3414,15 +3556,13 @@
         <v>0.79761688311688317</v>
       </c>
       <c r="M17" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.5770954611263833E-3</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="M19" s="24">
-        <f>AVERAGE(M12:M16)</f>
-        <v>2.0969088771799092E-3</v>
-      </c>
+      <c r="J19" s="29"/>
+      <c r="M19" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3434,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752A21F7-07F8-4DA3-997C-BEFBEAB2554C}">
   <dimension ref="B2:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,4 +4066,923 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9432D22C-8253-4384-BD4C-31624F09DD32}">
+  <dimension ref="B3:Q23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>134835</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.16081840539217701</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>162321</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.18439644336185801</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>107891</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.14390456124221801</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>270014</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.40203918014206003</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="39">
+        <f>AVERAGEIF($D$4:$D$21,I7,$F$4:$F$21)</f>
+        <v>0.20079153817770534</v>
+      </c>
+      <c r="K7" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="42">
+        <f>ABS(K7-J7)/K7</f>
+        <v>3.9576908885266548E-3</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>135055</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.16070111365263301</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="39">
+        <f>AVERAGEIF($D$4:$D$21,I8,$F$4:$F$21)</f>
+        <v>0.39962868827183667</v>
+      </c>
+      <c r="K8" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="L8" s="42">
+        <f t="shared" ref="L8:L12" si="0">ABS(K8-J8)/K8</f>
+        <v>9.2827932040837058E-4</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="1">
+        <v>538662</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.20115651172644899</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="39">
+        <f t="shared" ref="J9:J12" si="1">AVERAGEIF($D$4:$D$21,I9,$F$4:$F$21)</f>
+        <v>0.40061635879356006</v>
+      </c>
+      <c r="K9" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="L9" s="42">
+        <f t="shared" si="0"/>
+        <v>1.5408969839000863E-3</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>269558</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.395593121098338</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="39">
+        <f t="shared" si="1"/>
+        <v>0.16047011455506269</v>
+      </c>
+      <c r="K10" s="39">
+        <v>0.16</v>
+      </c>
+      <c r="L10" s="42">
+        <f t="shared" si="0"/>
+        <v>2.9382159691417747E-3</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="4">
+        <f>SUM(P5:P9)</f>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>270372</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.40396023860768898</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="39">
+        <f t="shared" si="1"/>
+        <v>0.18325019036754767</v>
+      </c>
+      <c r="K11" s="41">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="L11" s="42">
+        <f t="shared" si="0"/>
+        <v>7.8760470215121364E-3</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>108313</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.14268406710159601</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="39">
+        <f t="shared" si="1"/>
+        <v>0.14333017968435569</v>
+      </c>
+      <c r="K12" s="40">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="L12" s="43">
+        <f t="shared" si="0"/>
+        <v>3.3112577904898521E-3</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1">
+        <v>539934</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.202770166932906</v>
+      </c>
+      <c r="L13" s="44">
+        <f>AVERAGE(L7:L12)</f>
+        <v>3.4253979956631458E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>161621</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.182400424511172</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>268631</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.39776195033141698</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>270100</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.39288664606576101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="1">
+        <v>540546</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.198447935873761</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>270445</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.40849400495092503</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>134669</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.15989082462037801</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>107413</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.14340191070925301</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>162420</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.18295370322961299</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4899EA22-2C4E-460C-A0C9-CB4F1D5E0DA3}">
+  <dimension ref="B3:P21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>122827</v>
+      </c>
+      <c r="F4">
+        <v>0.15267966457721799</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>305772</v>
+      </c>
+      <c r="F5">
+        <v>0.65232860065481402</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>611297</v>
+      </c>
+      <c r="F6">
+        <v>0.336813996148144</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>305911</v>
+      </c>
+      <c r="F7">
+        <v>0.65234093008027505</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="39">
+        <f>AVERAGEIF($D$4:$D$21,I7,$F$4:$F$21)</f>
+        <v>0.33258320888107401</v>
+      </c>
+      <c r="K7" s="39">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L7" s="42">
+        <f>ABS(K7-J7)/K7</f>
+        <v>2.2503733567779127E-3</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>153158</v>
+      </c>
+      <c r="F8">
+        <v>0.17401876466268801</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="39">
+        <f>AVERAGEIF($D$4:$D$21,I8,$F$4:$F$21)</f>
+        <v>0.65160888586796872</v>
+      </c>
+      <c r="K8" s="39">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L8" s="42">
+        <f>ABS(K8-J8)/K8</f>
+        <v>2.2586671198046859E-2</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>122332</v>
+      </c>
+      <c r="F9">
+        <v>0.15034122748581799</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="39">
+        <f t="shared" ref="J8:J12" si="0">AVERAGEIF($D$4:$D$21,I9,$F$4:$F$21)</f>
+        <v>0.66299935203761362</v>
+      </c>
+      <c r="K9" s="39">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L9" s="42">
+        <f t="shared" ref="L8:L12" si="1">ABS(K9-J9)/K9</f>
+        <v>5.5009719435795135E-3</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>305368</v>
+      </c>
+      <c r="F10">
+        <v>0.65948749341572799</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="39">
+        <f t="shared" si="0"/>
+        <v>0.17384350634331799</v>
+      </c>
+      <c r="K10" s="39">
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="L10" s="42">
+        <f t="shared" si="1"/>
+        <v>3.9983852592150732E-4</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="4">
+        <f>SUM(P5:P9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>183285</v>
+      </c>
+      <c r="F11">
+        <v>0.20645602183828901</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="39">
+        <f t="shared" si="0"/>
+        <v>0.20506167117600269</v>
+      </c>
+      <c r="K11" s="39">
+        <v>0.2040816326530612</v>
+      </c>
+      <c r="L11" s="42">
+        <f t="shared" si="1"/>
+        <v>4.8021887624132738E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <v>611298</v>
+      </c>
+      <c r="F12">
+        <v>0.33143793328827398</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="39">
+        <f t="shared" si="0"/>
+        <v>0.15116467112537099</v>
+      </c>
+      <c r="K12" s="40">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="L12" s="43">
+        <f t="shared" si="1"/>
+        <v>2.3131705725514817E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>152751</v>
+      </c>
+      <c r="F13">
+        <v>0.17434693551081601</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="33">
+        <f>AVERAGE(L7:L12)</f>
+        <v>6.3088690598817583E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>183740</v>
+      </c>
+      <c r="F14">
+        <v>0.20377991304260001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>121719</v>
+      </c>
+      <c r="F15">
+        <v>0.150473121313077</v>
+      </c>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>306298</v>
+      </c>
+      <c r="F16">
+        <v>0.67746695327499296</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17">
+        <v>612400</v>
+      </c>
+      <c r="F17">
+        <v>0.329497697206804</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>306085</v>
+      </c>
+      <c r="F18">
+        <v>0.65015712686881699</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>152752</v>
+      </c>
+      <c r="F19">
+        <v>0.17316481885644999</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>183350</v>
+      </c>
+      <c r="F20">
+        <v>0.204949078647119</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>305524</v>
+      </c>
+      <c r="F21">
+        <v>0.65204360942212003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>